<commit_message>
Added more figure and data
</commit_message>
<xml_diff>
--- a/sims/s32/gs-radiances.xlsx
+++ b/sims/s32/gs-radiances.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="0" windowWidth="17640" windowHeight="14240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7260" yWindow="0" windowWidth="21060" windowHeight="18100" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="m0" sheetId="1" r:id="rId1"/>
+    <sheet name="m1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="gs_rad_tau0" localSheetId="0">Sheet1!$A$2:$C$22</definedName>
+    <definedName name="gs_rad_tau0" localSheetId="0">m0!$A$2:$C$22</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1146,7 +1146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>